<commit_message>
Updated for design changes
</commit_message>
<xml_diff>
--- a/PCB/PickAndPlace.xlsx
+++ b/PCB/PickAndPlace.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="PickAndPlace_PCB1_2024-11-30" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="PickAndPlace_PCB1_2024-12-13" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="81">
   <si>
     <t>Designator</t>
   </si>
@@ -64,13 +64,13 @@
     <t>SOD-323_L1.8-W1.3-LS2.5-RD</t>
   </si>
   <si>
-    <t>73.279mm</t>
-  </si>
-  <si>
-    <t>43.18mm</t>
-  </si>
-  <si>
-    <t>72.106mm</t>
+    <t>73.152mm</t>
+  </si>
+  <si>
+    <t>37.719mm</t>
+  </si>
+  <si>
+    <t>71.979mm</t>
   </si>
   <si>
     <t>T</t>
@@ -133,9 +133,6 @@
     <t>LED0805-RD_BLUE</t>
   </si>
   <si>
-    <t>73.152mm</t>
-  </si>
-  <si>
     <t>26.924mm</t>
   </si>
   <si>
@@ -193,16 +190,16 @@
     <t>RES-ARRAY-SMD_8P-L3.2-W1.6-P0.80-BL</t>
   </si>
   <si>
-    <t>72.991mm</t>
-  </si>
-  <si>
-    <t>38.036mm</t>
-  </si>
-  <si>
-    <t>73.761mm</t>
-  </si>
-  <si>
-    <t>36.686mm</t>
+    <t>73.406mm</t>
+  </si>
+  <si>
+    <t>42.799mm</t>
+  </si>
+  <si>
+    <t>74.176mm</t>
+  </si>
+  <si>
+    <t>41.449mm</t>
   </si>
   <si>
     <t>U1</t>
@@ -829,22 +826,22 @@
         <v>39</v>
       </c>
       <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="s">
         <v>40</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" t="s">
         <v>41</v>
-      </c>
-      <c r="F5" t="s">
-        <v>40</v>
-      </c>
-      <c r="G5" t="s">
-        <v>41</v>
-      </c>
-      <c r="H5" t="s">
-        <v>40</v>
-      </c>
-      <c r="I5" t="s">
-        <v>42</v>
       </c>
       <c r="J5">
         <v>2</v>
@@ -864,31 +861,31 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" t="s">
         <v>43</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>44</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
         <v>45</v>
       </c>
-      <c r="D6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" t="s">
         <v>46</v>
-      </c>
-      <c r="F6" t="s">
-        <v>40</v>
-      </c>
-      <c r="G6" t="s">
-        <v>46</v>
-      </c>
-      <c r="H6" t="s">
-        <v>40</v>
-      </c>
-      <c r="I6" t="s">
-        <v>47</v>
       </c>
       <c r="J6">
         <v>2</v>
@@ -903,36 +900,36 @@
         <v>21</v>
       </c>
       <c r="N6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" t="s">
         <v>49</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>50</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>51</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>52</v>
       </c>
-      <c r="E7" t="s">
-        <v>53</v>
-      </c>
       <c r="F7" t="s">
+        <v>51</v>
+      </c>
+      <c r="G7" t="s">
         <v>52</v>
       </c>
-      <c r="G7" t="s">
-        <v>53</v>
-      </c>
       <c r="H7" t="s">
+        <v>51</v>
+      </c>
+      <c r="I7" t="s">
         <v>52</v>
-      </c>
-      <c r="I7" t="s">
-        <v>53</v>
       </c>
       <c r="J7">
         <v>1</v>
@@ -947,12 +944,12 @@
         <v>21</v>
       </c>
       <c r="N7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B8" t="s">
         <v>24</v>
@@ -961,19 +958,19 @@
         <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E8" t="s">
         <v>27</v>
       </c>
       <c r="F8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G8" t="s">
         <v>27</v>
       </c>
       <c r="H8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I8" t="s">
         <v>29</v>
@@ -996,31 +993,31 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" t="s">
         <v>57</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>58</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>59</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>60</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9" t="s">
+        <v>60</v>
+      </c>
+      <c r="H9" t="s">
         <v>61</v>
       </c>
-      <c r="F9" t="s">
-        <v>60</v>
-      </c>
-      <c r="G9" t="s">
-        <v>61</v>
-      </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>62</v>
-      </c>
-      <c r="I9" t="s">
-        <v>63</v>
       </c>
       <c r="J9">
         <v>8</v>
@@ -1035,36 +1032,36 @@
         <v>21</v>
       </c>
       <c r="N9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" t="s">
         <v>64</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>65</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>66</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>67</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
+        <v>66</v>
+      </c>
+      <c r="G10" t="s">
+        <v>67</v>
+      </c>
+      <c r="H10" t="s">
         <v>68</v>
       </c>
-      <c r="F10" t="s">
-        <v>67</v>
-      </c>
-      <c r="G10" t="s">
-        <v>68</v>
-      </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>69</v>
-      </c>
-      <c r="I10" t="s">
-        <v>70</v>
       </c>
       <c r="J10">
         <v>23</v>
@@ -1079,36 +1076,36 @@
         <v>21</v>
       </c>
       <c r="N10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" t="s">
         <v>71</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>72</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>73</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>74</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
+        <v>73</v>
+      </c>
+      <c r="G11" t="s">
+        <v>74</v>
+      </c>
+      <c r="H11" t="s">
         <v>75</v>
       </c>
-      <c r="F11" t="s">
-        <v>74</v>
-      </c>
-      <c r="G11" t="s">
-        <v>75</v>
-      </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>76</v>
-      </c>
-      <c r="I11" t="s">
-        <v>77</v>
       </c>
       <c r="J11">
         <v>16</v>
@@ -1120,39 +1117,39 @@
         <v>90</v>
       </c>
       <c r="M11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="N11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" t="s">
         <v>79</v>
       </c>
-      <c r="B12" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" t="s">
-        <v>51</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>80</v>
       </c>
-      <c r="E12" t="s">
-        <v>81</v>
-      </c>
       <c r="F12" t="s">
+        <v>79</v>
+      </c>
+      <c r="G12" t="s">
         <v>80</v>
       </c>
-      <c r="G12" t="s">
-        <v>81</v>
-      </c>
       <c r="H12" t="s">
+        <v>79</v>
+      </c>
+      <c r="I12" t="s">
         <v>80</v>
-      </c>
-      <c r="I12" t="s">
-        <v>81</v>
       </c>
       <c r="J12">
         <v>1</v>
@@ -1167,7 +1164,7 @@
         <v>21</v>
       </c>
       <c r="N12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>